<commit_message>
chore: Adicionei uma coluna no Excel
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Barreto\Desktop\insert_to_postgresql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B9FFF3-DAB5-4BC9-A855-BCFDCB584437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621B5861-DA46-427A-91B5-092264457EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0E466FF2-DA99-4D1E-8343-4040C8BEF7C5}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$O$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$P$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="214">
   <si>
     <t>Cliente</t>
   </si>
@@ -615,9 +615,6 @@
     <t>004821111</t>
   </si>
   <si>
-    <t>FHD-626041-1</t>
-  </si>
-  <si>
     <t>74165</t>
   </si>
   <si>
@@ -636,9 +633,6 @@
     <t>status</t>
   </si>
   <si>
-    <t>traffic</t>
-  </si>
-  <si>
     <t>prefix</t>
   </si>
   <si>
@@ -679,13 +673,33 @@
   </si>
   <si>
     <t>terminal_id</t>
+  </si>
+  <si>
+    <r>
+      <t>traf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF242424"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>fic</t>
+    </r>
+  </si>
+  <si>
+    <t>HPT-626041-1</t>
+  </si>
+  <si>
+    <t>updated_at</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -725,6 +739,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF242424"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1144,84 +1164,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB9EA44C-88FB-42F1-A1FE-B510F30A9E34}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.77734375" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="16.5546875" defaultRowHeight="52.8" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:16" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>23</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="D2" s="4">
         <v>2</v>
@@ -1230,41 +1237,44 @@
         <v>1</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>200</v>
-      </c>
       <c r="H2" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="L2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="N2" s="6">
+        <v>55560</v>
+      </c>
+      <c r="O2" s="6">
+        <v>55380</v>
+      </c>
+      <c r="P2" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="M2" s="6">
-        <v>55560</v>
-      </c>
-      <c r="N2" s="6">
-        <v>55380</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:16" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O168" xr:uid="{BB9EA44C-88FB-42F1-A1FE-B510F30A9E34}"/>
+  <autoFilter ref="A1:P168" xr:uid="{BB9EA44C-88FB-42F1-A1FE-B510F30A9E34}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1275,7 +1285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0691870-B21E-4DF0-9C62-E2C3DB88349D}">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection sqref="A1:P37"/>
     </sheetView>
   </sheetViews>

</xml_diff>